<commit_message>
Update MATERIALI ATTESI_Dati esempio - Materiali attesi.xlsx
</commit_message>
<xml_diff>
--- a/examples/it/MATERIALI ATTESI_Dati esempio - Materiali attesi.xlsx
+++ b/examples/it/MATERIALI ATTESI_Dati esempio - Materiali attesi.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">MI</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA003</t>
+    <t xml:space="preserve">MIGA001</t>
   </si>
   <si>
     <t xml:space="preserve">Tende</t>
@@ -85,13 +85,13 @@
     <t xml:space="preserve">ORG0001</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA004</t>
+    <t xml:space="preserve">MIGA002</t>
   </si>
   <si>
     <t xml:space="preserve">A.V. STIACCINO</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA005</t>
+    <t xml:space="preserve">MIGA003</t>
   </si>
   <si>
     <t xml:space="preserve">GAZEBO MT6 X 3 COMPLETO</t>
@@ -100,49 +100,49 @@
     <t xml:space="preserve">ORG0002</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRGA007</t>
+    <t xml:space="preserve">MIGA004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIGA005</t>
   </si>
   <si>
     <t xml:space="preserve">A.V. SUCCIACAPRE</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA008</t>
+    <t xml:space="preserve">MIGA006</t>
   </si>
   <si>
     <t xml:space="preserve">ORG0003</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA009</t>
+    <t xml:space="preserve">MIGA007</t>
   </si>
   <si>
     <t xml:space="preserve">GAZEBO MT 3 X 3 CON PARETI</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRGA011</t>
+    <t xml:space="preserve">MIGA008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIGA009</t>
   </si>
   <si>
     <t xml:space="preserve">A.V. TARABUSINO</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA012</t>
+    <t xml:space="preserve">MIGA010</t>
   </si>
   <si>
     <t xml:space="preserve">ORG0004</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA017</t>
+    <t xml:space="preserve">MIGA011</t>
   </si>
   <si>
     <t xml:space="preserve">A.V. TORDO SASSELLO</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA016</t>
+    <t xml:space="preserve">MIGA012</t>
   </si>
   <si>
     <t xml:space="preserve">ORG0005</t>
@@ -151,31 +151,31 @@
     <t xml:space="preserve">A.V. USIGNOLO</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA015</t>
+    <t xml:space="preserve">MIGA013</t>
   </si>
   <si>
     <t xml:space="preserve">ORG0006</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA001</t>
+    <t xml:space="preserve">MIGA014</t>
   </si>
   <si>
     <t xml:space="preserve">A.V. VOLTAPIETRE</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA002</t>
+    <t xml:space="preserve">MIGA015</t>
   </si>
   <si>
     <t xml:space="preserve">ORG0007</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA014</t>
+    <t xml:space="preserve">MIGA016</t>
   </si>
   <si>
     <t xml:space="preserve">A.V. ZIGOLO MUCIATTO</t>
   </si>
   <si>
-    <t xml:space="preserve">CRGA013</t>
+    <t xml:space="preserve">MIGA017</t>
   </si>
   <si>
     <t xml:space="preserve">ORG0008</t>
@@ -254,8 +254,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -454,556 +458,556 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="0" t="s">
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="0" t="s">
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="0" t="s">
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="0" t="s">
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="0" t="s">
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="0" t="s">
+      <c r="G9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="0" t="s">
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="0" t="s">
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="0" t="s">
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="0" t="s">
+      <c r="G13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="0" t="s">
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="0" t="s">
+      <c r="G15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="0" t="s">
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="0" t="s">
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="0" t="s">
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>